<commit_message>
Nicht ganz wie geplant
</commit_message>
<xml_diff>
--- a/KM_test/src/resources/zeitplan/Zeitplan.xlsx
+++ b/KM_test/src/resources/zeitplan/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="21315" windowHeight="8250"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19200" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Truppen &amp; GUI Probleme behoben</t>
   </si>
@@ -387,14 +388,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -423,9 +421,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -443,6 +438,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -759,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -784,18 +782,18 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>42150</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <f>B3+1+F10</f>
         <v>42151</v>
       </c>
@@ -807,7 +805,7 @@
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <f t="shared" ref="B5:B44" si="0">B4+1+F11</f>
         <v>42152</v>
       </c>
@@ -819,11 +817,11 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <f t="shared" si="0"/>
         <v>42153</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
@@ -831,73 +829,75 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <f t="shared" si="0"/>
         <v>42154</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <f t="shared" si="0"/>
         <v>42155</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <f t="shared" si="0"/>
         <v>42156</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <f t="shared" si="0"/>
         <v>42157</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <f>COUNTIF(D3:D44, "nein")</f>
         <v>0</v>
       </c>
-      <c r="G10" s="8" t="str">
+      <c r="G10" s="7" t="str">
         <f>IF(F10 = 1, "Tag", "Tage")</f>
         <v>Tage</v>
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <f t="shared" si="0"/>
         <v>42158</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <f t="shared" si="0"/>
         <v>42159</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <f t="shared" si="0"/>
         <v>42160</v>
       </c>
@@ -906,7 +906,7 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <f t="shared" si="0"/>
         <v>42161</v>
       </c>
@@ -915,65 +915,65 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <f t="shared" si="0"/>
         <v>42162</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <f t="shared" si="0"/>
         <v>42163</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <f t="shared" si="0"/>
         <v>42164</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <f t="shared" si="0"/>
         <v>42165</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <f t="shared" si="0"/>
         <v>42166</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <f t="shared" si="0"/>
         <v>42167</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" spans="2:3">
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <f t="shared" si="0"/>
         <v>42168</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" spans="2:3">
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <f t="shared" si="0"/>
         <v>42169</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" spans="2:3">
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <f t="shared" si="0"/>
         <v>42170</v>
       </c>
@@ -982,7 +982,7 @@
       </c>
     </row>
     <row r="24" spans="2:3">
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <f t="shared" si="0"/>
         <v>42171</v>
       </c>
@@ -991,146 +991,146 @@
       </c>
     </row>
     <row r="25" spans="2:3">
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <f t="shared" si="0"/>
         <v>42172</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <f t="shared" si="0"/>
         <v>42173</v>
       </c>
-      <c r="C26" s="19"/>
+      <c r="C26" s="17"/>
     </row>
     <row r="27" spans="2:3">
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <f t="shared" si="0"/>
         <v>42174</v>
       </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="17"/>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <f t="shared" si="0"/>
         <v>42175</v>
       </c>
-      <c r="C28" s="19"/>
+      <c r="C28" s="17"/>
     </row>
     <row r="29" spans="2:3">
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <f t="shared" si="0"/>
         <v>42176</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="17"/>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <f t="shared" si="0"/>
         <v>42177</v>
       </c>
-      <c r="C30" s="19"/>
+      <c r="C30" s="17"/>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <f t="shared" si="0"/>
         <v>42178</v>
       </c>
-      <c r="C31" s="19"/>
+      <c r="C31" s="17"/>
     </row>
     <row r="32" spans="2:3">
-      <c r="B32" s="10">
+      <c r="B32" s="9">
         <f t="shared" si="0"/>
         <v>42179</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="17"/>
     </row>
     <row r="33" spans="2:3">
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <f t="shared" si="0"/>
         <v>42180</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="17"/>
     </row>
     <row r="34" spans="2:3">
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <f t="shared" si="0"/>
         <v>42181</v>
       </c>
-      <c r="C34" s="19"/>
+      <c r="C34" s="17"/>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="10">
+      <c r="B35" s="9">
         <f t="shared" si="0"/>
         <v>42182</v>
       </c>
-      <c r="C35" s="19"/>
+      <c r="C35" s="17"/>
     </row>
     <row r="36" spans="2:3">
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <f t="shared" si="0"/>
         <v>42183</v>
       </c>
-      <c r="C36" s="19"/>
+      <c r="C36" s="17"/>
     </row>
     <row r="37" spans="2:3">
-      <c r="B37" s="10">
+      <c r="B37" s="9">
         <f t="shared" si="0"/>
         <v>42184</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="17"/>
     </row>
     <row r="38" spans="2:3">
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <f t="shared" si="0"/>
         <v>42185</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="17"/>
     </row>
     <row r="39" spans="2:3">
-      <c r="B39" s="10">
+      <c r="B39" s="9">
         <f t="shared" si="0"/>
         <v>42186</v>
       </c>
-      <c r="C39" s="19"/>
+      <c r="C39" s="17"/>
     </row>
     <row r="40" spans="2:3">
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <f t="shared" si="0"/>
         <v>42187</v>
       </c>
-      <c r="C40" s="19"/>
+      <c r="C40" s="17"/>
     </row>
     <row r="41" spans="2:3">
-      <c r="B41" s="10">
+      <c r="B41" s="9">
         <f t="shared" si="0"/>
         <v>42188</v>
       </c>
-      <c r="C41" s="19"/>
+      <c r="C41" s="17"/>
     </row>
     <row r="42" spans="2:3">
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <f t="shared" si="0"/>
         <v>42189</v>
       </c>
-      <c r="C42" s="19"/>
+      <c r="C42" s="17"/>
     </row>
     <row r="43" spans="2:3">
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <f t="shared" si="0"/>
         <v>42190</v>
       </c>
-      <c r="C43" s="20"/>
+      <c r="C43" s="18"/>
     </row>
     <row r="44" spans="2:3" ht="92.25">
-      <c r="B44" s="11">
+      <c r="B44" s="10">
         <f t="shared" si="0"/>
         <v>42191</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="22" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>